<commit_message>
regression data table test 1
</commit_message>
<xml_diff>
--- a/DataTables/Book2.xlsx
+++ b/DataTables/Book2.xlsx
@@ -36,13 +36,13 @@
     <t>c</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
-    <t>f</t>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>d2</t>
   </si>
 </sst>
 </file>
@@ -364,7 +364,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,15 +382,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>